<commit_message>
Updated QQ logs and QQ Route bug fix in ejs file which was redirecting to Master route
</commit_message>
<xml_diff>
--- a/public/download/sample-dncfile.xlsx
+++ b/public/download/sample-dncfile.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prajwal.pawar\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shoaib.Mulani\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36E467A-F207-4B72-B20E-6F45270AD87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30631DA-77C1-4410-A22A-395A7DF8C607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43CD9620-56BD-4382-B15A-A487C33BA1F2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{43CD9620-56BD-4382-B15A-A487C33BA1F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Email ID</t>
   </si>
@@ -45,6 +34,12 @@
   </si>
   <si>
     <t>Domain</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
   </si>
 </sst>
 </file>
@@ -416,24 +411,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D01688-C2BE-44DF-B581-EF373F8F6F9C}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>